<commit_message>
Fix incorrect part numbers
</commit_message>
<xml_diff>
--- a/Source/Project Outputs for RUMBA_plus/RUMBA_plus_BOM_1_4_0.xlsx
+++ b/Source/Project Outputs for RUMBA_plus/RUMBA_plus_BOM_1_4_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Git\RUMBA-Plus\Source\Project Outputs for RUMBA_plus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7F46EB-38FF-4F9F-9089-744BB2B77299}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE203C03-169D-4A22-9D03-B44C695E5F42}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22275" windowHeight="16230" xr2:uid="{FD7B852F-20E6-4A44-AE1F-F610DC299137}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{FD7B852F-20E6-4A44-AE1F-F610DC299137}"/>
   </bookViews>
   <sheets>
     <sheet name="RUMBA_plus_BOM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="264">
   <si>
     <t>Designator</t>
   </si>
@@ -570,12 +570,6 @@
     <t>348K</t>
   </si>
   <si>
-    <t>RC0603FR-0753K6L</t>
-  </si>
-  <si>
-    <t>311-53.6KHRCT-ND</t>
-  </si>
-  <si>
     <t>R40, R41, R42, R43, R54, R59</t>
   </si>
   <si>
@@ -802,6 +796,27 @@
   </si>
   <si>
     <t>277-6405-ND</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <t>C0603C272K5RACTU</t>
+  </si>
+  <si>
+    <t>399-7890-1-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07348KL</t>
+  </si>
+  <si>
+    <t>311-348KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0754K9L</t>
+  </si>
+  <si>
+    <t>311-54.9KHRCT-ND</t>
   </si>
 </sst>
 </file>
@@ -1427,7 +1442,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{453F7D77-1F44-4C69-BB8E-A7C089CDC468}" name="Table1" displayName="Table1" ref="A1:J50" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A1:J50" xr:uid="{65A4A817-A6AE-4425-AE9B-B9C2B3F0E384}"/>
-  <sortState ref="A2:J50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J50">
     <sortCondition ref="A1:A50"/>
   </sortState>
   <tableColumns count="10">
@@ -1745,8 +1760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A98E15-2981-43F2-B0A5-2FE7530EB2D1}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,7 +1830,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="1"/>
@@ -1858,7 +1873,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -1873,16 +1888,16 @@
         <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>32</v>
+        <v>257</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>33</v>
+        <v>258</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>34</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1890,7 +1905,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>45</v>
@@ -1922,7 +1937,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>24</v>
@@ -1954,7 +1969,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -1986,7 +2001,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>36</v>
@@ -2082,7 +2097,7 @@
         <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>65</v>
@@ -2114,7 +2129,7 @@
         <v>69</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>70</v>
@@ -2146,13 +2161,13 @@
         <v>73</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -2161,27 +2176,27 @@
         <v>14</v>
       </c>
       <c r="G13" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -2193,7 +2208,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="1"/>
@@ -2233,7 +2248,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>80</v>
@@ -2251,7 +2266,7 @@
         <v>14</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
@@ -2309,7 +2324,7 @@
         <v>14</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="1"/>
@@ -2335,7 +2350,7 @@
         <v>14</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="1"/>
@@ -2455,13 +2470,13 @@
         <v>77</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2484,7 +2499,7 @@
         <v>14</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
@@ -2525,7 +2540,7 @@
         <v>122</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>124</v>
@@ -2682,13 +2697,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2">
@@ -2696,24 +2711,24 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>149</v>
@@ -2728,16 +2743,16 @@
         <v>13</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2827,13 +2842,13 @@
         <v>32</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>182</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2902,16 +2917,16 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E38" s="2">
         <v>6</v>
@@ -2923,13 +2938,13 @@
         <v>32</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2955,27 +2970,27 @@
         <v>32</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>160</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E40" s="2">
         <v>1</v>
@@ -2998,7 +3013,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>151</v>
@@ -3030,13 +3045,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -3048,27 +3063,27 @@
         <v>14</v>
       </c>
       <c r="G42" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -3080,27 +3095,27 @@
         <v>13</v>
       </c>
       <c r="G43" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -3112,27 +3127,27 @@
         <v>13</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -3144,27 +3159,27 @@
         <v>13</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -3176,27 +3191,27 @@
         <v>13</v>
       </c>
       <c r="G46" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -3208,21 +3223,21 @@
         <v>14</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H47" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>112</v>
@@ -3240,7 +3255,7 @@
         <v>14</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="1"/>
@@ -3248,13 +3263,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
@@ -3266,7 +3281,7 @@
         <v>14</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="1"/>
@@ -3274,13 +3289,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C50" s="11" t="s">
         <v>222</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>224</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>13</v>
@@ -3292,16 +3307,16 @@
         <v>14</v>
       </c>
       <c r="G50" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50" s="14" t="s">
         <v>225</v>
-      </c>
-      <c r="H50" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J50" s="14" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3320,121 +3335,115 @@
     <hyperlink ref="H8" r:id="rId12" tooltip="Manufacturer" display="'06035C220JAT2A" xr:uid="{47EA9C31-BDE5-4D4F-ACF8-DE3F56E9D72B}"/>
     <hyperlink ref="J8" r:id="rId13" tooltip="Supplier" display="'478-6204-1-ND" xr:uid="{FDD5D832-74CB-4683-A2DB-D972C4C1908C}"/>
     <hyperlink ref="G4" r:id="rId14" tooltip="Component" display="'Yageo" xr:uid="{4E49C13C-91A0-4CA8-8CE3-A65BF95CC3A7}"/>
-    <hyperlink ref="H4" r:id="rId15" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{6D1B755B-7D86-4DE3-B171-CC6E411A442B}"/>
-    <hyperlink ref="J4" r:id="rId16" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{5B8E0970-0B4A-4EE1-8FD7-28106AD83EA0}"/>
-    <hyperlink ref="G5" r:id="rId17" tooltip="Component" display="'Murata Electronics North America" xr:uid="{E7F5D5C7-EA41-4AA5-9366-4053E4BA72B3}"/>
-    <hyperlink ref="H5" r:id="rId18" tooltip="Manufacturer" display="'GRM32ER71H475KA88L" xr:uid="{A6EDC89B-1ED0-4754-9FF8-669DA8AF9522}"/>
-    <hyperlink ref="J5" r:id="rId19" tooltip="Supplier" display="'490-1864-1-ND" xr:uid="{A5AB9FC1-6372-4527-B577-FAA610CCDA97}"/>
-    <hyperlink ref="G9" r:id="rId20" tooltip="Component" display="'Diodes Inc" xr:uid="{2B3BD86C-29DA-46F2-8BAB-496617D12C1D}"/>
-    <hyperlink ref="H9" r:id="rId21" tooltip="Manufacturer" display="'S2BA-13-F" xr:uid="{28D5A782-892D-4B5B-8380-049E4BA9F589}"/>
-    <hyperlink ref="J9" r:id="rId22" tooltip="Supplier" display="'S2BA-FDICT-ND" xr:uid="{3F6CB655-0A7A-4880-A499-C0D848DB5627}"/>
-    <hyperlink ref="G10" r:id="rId23" tooltip="Component" display="'Micro Commercial Co" xr:uid="{0ABF9B14-67E4-403C-BC40-1631C6627605}"/>
-    <hyperlink ref="H10" r:id="rId24" tooltip="Manufacturer" display="'1N4148WX-TP" xr:uid="{E6239A4B-5131-49CD-92C9-030E55C8AD2E}"/>
-    <hyperlink ref="J10" r:id="rId25" tooltip="Supplier" display="'1N4148WXTPMSCT-ND" xr:uid="{4CBDC6BE-E0DC-495F-82C3-C420312D1A34}"/>
-    <hyperlink ref="G11" r:id="rId26" tooltip="Component" display="'Nexperia USA Inc." xr:uid="{1F61F94C-3850-4235-BC0F-EB9AD2F10894}"/>
-    <hyperlink ref="H11" r:id="rId27" tooltip="Manufacturer" display="'PMEG2020CPA,115" xr:uid="{0647B961-D44E-4662-B585-05AB6FA8A2CD}"/>
-    <hyperlink ref="J11" r:id="rId28" tooltip="Supplier" display="'1727-5194-1-ND" xr:uid="{25EBC6D0-7FBE-4D7E-8B6E-D589DB20F252}"/>
-    <hyperlink ref="G12" r:id="rId29" tooltip="Component" display="'Panasonic Electronic Components" xr:uid="{8E3BD2BA-DB6B-4FF3-A478-ACA69833B264}"/>
-    <hyperlink ref="H12" r:id="rId30" tooltip="Manufacturer" display="'DB2W40200L" xr:uid="{3761DF13-7813-4DFB-BC75-D47D9A3F904A}"/>
-    <hyperlink ref="J12" r:id="rId31" tooltip="Supplier" display="'DB2W40200LCT-ND" xr:uid="{48AE65F7-B989-4848-9591-2634A67A76AC}"/>
-    <hyperlink ref="G13" r:id="rId32" tooltip="Component" display="'SMC Diode Solutions" xr:uid="{AC22599F-B23D-4E43-AF11-EA72A9730063}"/>
-    <hyperlink ref="H13" r:id="rId33" tooltip="Manufacturer" display="'SK520BTR" xr:uid="{97298E20-975B-4CC3-8E21-71A6D4210AF9}"/>
-    <hyperlink ref="G14" r:id="rId34" tooltip="Component" display="'Sullins Connector Solutions" xr:uid="{F5FC59FA-9C19-4224-A7E5-E0FFF0CF83FE}"/>
-    <hyperlink ref="G15" r:id="rId35" tooltip="Component" display="'Phoenix Contact" xr:uid="{4766C111-E58E-4CDE-8EC1-5FBC0179B5E5}"/>
-    <hyperlink ref="H15" r:id="rId36" tooltip="Manufacturer" display="'1751264" xr:uid="{D31C62C5-0E89-49F5-9999-F164C1E7A95C}"/>
-    <hyperlink ref="J15" r:id="rId37" tooltip="Supplier" display="'277-5744-ND" xr:uid="{80E17885-8837-4CE3-93A1-C275271B3970}"/>
-    <hyperlink ref="G16" r:id="rId38" tooltip="Component" display="'Loading..." xr:uid="{DDFEE7F0-F3D2-4DC8-AE6C-7EAA9AFB0567}"/>
-    <hyperlink ref="G17" r:id="rId39" tooltip="Component" display="'Wurth Electronics Inc." xr:uid="{9C34FDB8-BE7F-40A9-9310-6F4073CE0FDF}"/>
-    <hyperlink ref="H17" r:id="rId40" tooltip="Manufacturer" display="'416131160803" xr:uid="{EC87D714-1A5E-4268-AF35-62693127FE37}"/>
-    <hyperlink ref="J17" r:id="rId41" tooltip="Supplier" display="'732-3853-1-ND" xr:uid="{87EF3683-C2E7-473B-868A-3A631DD27E52}"/>
-    <hyperlink ref="G18" r:id="rId42" tooltip="Component" display="'Loading..." xr:uid="{0A8E1813-F956-4A5B-8D10-B8DB52FDDBE4}"/>
-    <hyperlink ref="G19" r:id="rId43" tooltip="Component" display="'3M" xr:uid="{68CD3745-038B-4380-81BA-87034167EE3C}"/>
-    <hyperlink ref="G20" r:id="rId44" tooltip="Component" display="'MPD (Memory Protection Devices)" xr:uid="{FE298821-F0A5-4495-958A-5F81A2E04060}"/>
-    <hyperlink ref="H20" r:id="rId45" tooltip="Manufacturer" display="'BK-6013" xr:uid="{0F8C2023-4819-4C0C-B171-33CEE13AE4A6}"/>
-    <hyperlink ref="J20" r:id="rId46" tooltip="Supplier" display="'BK-6013-ND" xr:uid="{E61A265C-62CB-4F2B-942B-0CA0AF6703E9}"/>
-    <hyperlink ref="G21" r:id="rId47" tooltip="Component" display="'Holly Fuse" xr:uid="{0C8965CF-A757-4F40-A8B2-FD40A4E8C193}"/>
-    <hyperlink ref="H21" r:id="rId48" tooltip="Manufacturer" display="'06T-0160L" xr:uid="{87AB65B0-3F61-4B4B-BB53-75CD15E64701}"/>
-    <hyperlink ref="J21" r:id="rId49" tooltip="Supplier" display="'507-1821-1-ND" xr:uid="{EDCE14BF-745A-4FC1-B9D4-E74525915207}"/>
-    <hyperlink ref="G22" r:id="rId50" tooltip="Component" display="'Phoenix Contact" xr:uid="{8E33D070-85B3-45B0-9D72-9DEA8C64A27A}"/>
-    <hyperlink ref="H22" r:id="rId51" tooltip="Manufacturer" display="'1751248" xr:uid="{27069FCF-26AC-4F60-8EDA-B73F085A841F}"/>
-    <hyperlink ref="J22" r:id="rId52" tooltip="Supplier" display="'277-5719-ND" xr:uid="{072D2A82-ED4A-4927-B341-58FB066FBA76}"/>
-    <hyperlink ref="G48" r:id="rId53" tooltip="Component" display="'Loading..." xr:uid="{99534DDB-1774-407E-BD72-7D3668C9B630}"/>
-    <hyperlink ref="G24" r:id="rId54" tooltip="Component" display="'Loading..." xr:uid="{D760A977-B9E1-4C61-8FAE-CB62F2BEFBBD}"/>
-    <hyperlink ref="G25" r:id="rId55" tooltip="Component" display="'Molex, LLC" xr:uid="{0F5FD788-F564-4A60-A2B5-109732D6ED30}"/>
-    <hyperlink ref="H25" r:id="rId56" tooltip="Manufacturer" display="'1050170001" xr:uid="{B10606C0-E169-41AC-9B1B-F046E7E8510B}"/>
-    <hyperlink ref="J25" r:id="rId57" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{0989CB1B-579D-4020-A5FD-0E4ABE9D7703}"/>
-    <hyperlink ref="G26" r:id="rId58" tooltip="Component" display="'Murata Electronics North America" xr:uid="{D4304DAD-AEA9-4A0B-9023-C8C19E9FD2F3}"/>
-    <hyperlink ref="H26" r:id="rId59" tooltip="Manufacturer" display="'BLM21PG221SN1D" xr:uid="{63933F83-B76B-44CD-8CE8-1865C9C817D7}"/>
-    <hyperlink ref="J26" r:id="rId60" tooltip="Supplier" display="'490-1054-1-ND" xr:uid="{1E4D4793-B327-43AA-8F6C-D834CE45C90D}"/>
-    <hyperlink ref="G27" r:id="rId61" tooltip="Component" display="'Bourns Inc." xr:uid="{5E42FB16-A764-47DE-9A5B-D5B7FB62B66C}"/>
-    <hyperlink ref="H27" r:id="rId62" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{2CD86F8E-580A-44C3-A25C-C9769E024EF7}"/>
-    <hyperlink ref="J27" r:id="rId63" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{13951AE0-C7C0-43BA-BE32-C42CFD079DC4}"/>
-    <hyperlink ref="G28" r:id="rId64" tooltip="Component" display="'Bourns Inc." xr:uid="{3A3BA2F0-D76C-4591-8243-99CD334215D0}"/>
-    <hyperlink ref="H28" r:id="rId65" tooltip="Manufacturer" display="'SRN8040TA-470M" xr:uid="{9393FD5F-F406-4DDA-B2F6-A5087E59B162}"/>
-    <hyperlink ref="J28" r:id="rId66" tooltip="Supplier" display="'SRN8040TA-470MCT-ND" xr:uid="{BE956B5E-DBA7-4876-99D7-BD2953EE7A3E}"/>
-    <hyperlink ref="G29" r:id="rId67" tooltip="Component" display="'Lite-On Inc." xr:uid="{1BFC70D3-D369-4F4A-BC39-F51EC41C90E5}"/>
-    <hyperlink ref="H29" r:id="rId68" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{961D9B5D-F3D3-46C6-9E7D-993401706C55}"/>
-    <hyperlink ref="J29" r:id="rId69" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{4989D82B-EDE2-45AD-8316-0BE497E40D5B}"/>
-    <hyperlink ref="G30" r:id="rId70" tooltip="Component" display="'Lite-On Inc." xr:uid="{639D4ACD-5799-402D-803C-17A777CAFADE}"/>
-    <hyperlink ref="H30" r:id="rId71" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{2413BFA6-6008-41BC-AB9E-D0CADB0841F0}"/>
-    <hyperlink ref="J30" r:id="rId72" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{94979B37-F572-4850-BEF9-C3428194D2AD}"/>
-    <hyperlink ref="G33" r:id="rId73" tooltip="Component" display="'Yageo" xr:uid="{08B992B2-5FFD-468F-8C37-F5E0E55827CA}"/>
-    <hyperlink ref="H33" r:id="rId74" tooltip="Manufacturer" display="'RC0603FR-071ML" xr:uid="{7D006478-1E4D-4D42-85C7-033ABCB72197}"/>
-    <hyperlink ref="J33" r:id="rId75" tooltip="Supplier" display="'311-1.00MHRDKR-ND" xr:uid="{85B8248E-2152-4AEE-9145-234BD60567AA}"/>
-    <hyperlink ref="G36" r:id="rId76" tooltip="Component" display="'Yageo" xr:uid="{7A3BC117-10FA-4978-95C8-B8FEC528AE8C}"/>
-    <hyperlink ref="H36" r:id="rId77" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{3E10DF3F-5206-4953-A38F-24F8BF7A0D63}"/>
-    <hyperlink ref="J36" r:id="rId78" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{6A20EF17-382F-49C2-A769-EBF46975E659}"/>
-    <hyperlink ref="G37" r:id="rId79" tooltip="Component" display="'Yageo" xr:uid="{5F9D81C6-4FA4-41B4-83FC-838B41BF9D63}"/>
-    <hyperlink ref="H37" r:id="rId80" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{EC5C9DBC-CA01-4E84-8AB1-A1E011F4969C}"/>
-    <hyperlink ref="J37" r:id="rId81" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{9EE26DE7-963D-4581-A9CD-06D42E170F76}"/>
-    <hyperlink ref="G39" r:id="rId82" tooltip="Component" display="'Yageo" xr:uid="{7CC16B12-D4DA-42BE-B00E-AF45B84234CE}"/>
-    <hyperlink ref="H39" r:id="rId83" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{4B29041A-5D4F-4E9F-85F0-FE3EC9EECF7F}"/>
-    <hyperlink ref="J39" r:id="rId84" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{91882D23-815E-4187-9AAD-24127BF44ECE}"/>
-    <hyperlink ref="G41" r:id="rId85" tooltip="Component" display="'Yageo" xr:uid="{14BC76A9-9358-431A-80A8-D0CD2925110D}"/>
-    <hyperlink ref="H41" r:id="rId86" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{0C32B3D1-D5BC-425A-9128-C60912E9D570}"/>
-    <hyperlink ref="J41" r:id="rId87" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{F851E52C-EEB8-4A75-9E50-490FA833C07A}"/>
-    <hyperlink ref="G34" r:id="rId88" tooltip="Component" display="'Yageo" xr:uid="{04DAF956-9707-421B-9902-660D148AD02A}"/>
-    <hyperlink ref="H34" r:id="rId89" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{8885096B-1925-40B5-9B6A-8A913F04A0E5}"/>
-    <hyperlink ref="J34" r:id="rId90" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{008657BB-878C-496B-AC2C-CAF672731554}"/>
-    <hyperlink ref="G35" r:id="rId91" tooltip="Component" display="'Yageo" xr:uid="{2FBCF6ED-10E7-4215-9E32-249EF6E45BAE}"/>
-    <hyperlink ref="H35" r:id="rId92" tooltip="Manufacturer" display="'RC0603FR-0753K6L" xr:uid="{D20F714A-064B-47F9-A242-40BB25004199}"/>
-    <hyperlink ref="J35" r:id="rId93" tooltip="Supplier" display="'311-53.6KHRCT-ND" xr:uid="{B0FC8B5D-3CA9-41D6-978F-C4C739948B27}"/>
-    <hyperlink ref="G38" r:id="rId94" tooltip="Component" display="'Yageo" xr:uid="{D05D8D23-0FD7-4EB0-82B5-012867FB4A29}"/>
-    <hyperlink ref="H38" r:id="rId95" tooltip="Manufacturer" display="'RC0603JR-074K7L" xr:uid="{487CC820-6958-4015-8E07-2B1B6917AB28}"/>
-    <hyperlink ref="J38" r:id="rId96" tooltip="Supplier" display="'311-4.7KGRCT-ND" xr:uid="{EB3C4C30-1438-46A2-85B2-C2570D6C8061}"/>
-    <hyperlink ref="G40" r:id="rId97" tooltip="Component" display="'Yageo" xr:uid="{83B23BCD-9D2D-4244-A8D9-855CBC334E2E}"/>
-    <hyperlink ref="H40" r:id="rId98" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{CC682DC2-92DA-4617-89AC-DBE9484E8EB3}"/>
-    <hyperlink ref="J40" r:id="rId99" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{77F80A98-4E5F-42FB-8366-09D154AF8FBF}"/>
-    <hyperlink ref="G42" r:id="rId100" tooltip="Component" display="'APEM Inc." xr:uid="{8DA80FE1-AD41-41A1-AF5B-29C7AE5C205A}"/>
-    <hyperlink ref="H42" r:id="rId101" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{3E38DB83-F083-4406-9B4E-413981B63A75}"/>
-    <hyperlink ref="J42" r:id="rId102" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{801CE691-B5ED-4969-8922-A4400E0A0F04}"/>
-    <hyperlink ref="G46" r:id="rId103" tooltip="Component" display="'Alpha &amp; Omega Semiconductor Inc." xr:uid="{B20D082B-86E0-455B-948A-E56AA2128005}"/>
-    <hyperlink ref="H46" r:id="rId104" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{FBD90C73-9CDC-45FA-A900-851BCE6704DB}"/>
-    <hyperlink ref="J46" r:id="rId105" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{E2C42AC0-6C55-40A7-8049-274675441D9B}"/>
-    <hyperlink ref="G47" r:id="rId106" tooltip="Component" display="'STMicroelectronics" xr:uid="{785209C2-D378-474E-97B4-42C17DE72E9A}"/>
-    <hyperlink ref="H47" r:id="rId107" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{98791FDC-D4C5-4551-847A-1B45F6539CBF}"/>
-    <hyperlink ref="J47" r:id="rId108" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{E2F9A172-96B8-4383-B884-A6A1414CF4A7}"/>
-    <hyperlink ref="G43" r:id="rId109" tooltip="Component" display="'Microchip Technology" xr:uid="{D0D2B9E1-7600-421F-BB55-D5E4CF817D2B}"/>
-    <hyperlink ref="H43" r:id="rId110" tooltip="Manufacturer" display="'ATMEGA2560-16AU" xr:uid="{3090BB5A-0847-4847-AA65-518ED9057C4F}"/>
-    <hyperlink ref="J43" r:id="rId111" tooltip="Supplier" display="'ATMEGA2560-16AU-ND" xr:uid="{21D45919-A9D2-4071-80EE-68A0A0D8492D}"/>
-    <hyperlink ref="G44" r:id="rId112" tooltip="Component" display="'Microchip Technology" xr:uid="{21BB9AC5-9AC5-4C89-A6B2-5C2DD94EEA56}"/>
-    <hyperlink ref="H44" r:id="rId113" tooltip="Manufacturer" display="'ATMEGA16U2-AU" xr:uid="{71DEC28B-A006-4DF5-BB66-FBB703DC7EFC}"/>
-    <hyperlink ref="J44" r:id="rId114" tooltip="Supplier" display="'ATMEGA16U2-AU-ND" xr:uid="{752CFA2A-364D-4706-BD90-0EF7750AEE11}"/>
-    <hyperlink ref="G45" r:id="rId115" tooltip="Component" display="'Alpha &amp; Omega Semiconductor Inc." xr:uid="{BE4F2880-1B87-45DB-B4B9-3BC68B11948D}"/>
-    <hyperlink ref="H45" r:id="rId116" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{00CF3BA0-9B64-4C44-A4CC-99B3C12958E9}"/>
-    <hyperlink ref="J45" r:id="rId117" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{CE07DCE4-81F1-4E37-AE55-1FF5C4A25DD5}"/>
-    <hyperlink ref="G49" r:id="rId118" tooltip="Component" display="'Loading..." xr:uid="{7FFD9829-C7FD-48AB-9008-67414D5F3A9B}"/>
-    <hyperlink ref="G50" r:id="rId119" tooltip="Component" display="'EPSON" xr:uid="{307A7C81-BA6D-4A04-84C8-3CD77AE1DB8E}"/>
-    <hyperlink ref="H50" r:id="rId120" tooltip="Manufacturer" display="'FA-238 16.0000MB-C3" xr:uid="{38323FE7-4E4F-4998-8A1E-5F7113325831}"/>
-    <hyperlink ref="J50" r:id="rId121" tooltip="Supplier" display="'SER3686CT-ND" xr:uid="{225B874A-BB17-40EC-AD86-2ADBDA9439C8}"/>
-    <hyperlink ref="G32" r:id="rId122" tooltip="Component" xr:uid="{8C0B0BB1-B33C-4761-A4B1-3E86C1AAAB94}"/>
-    <hyperlink ref="H32" r:id="rId123" tooltip="Manufacturer" xr:uid="{6F8EF1F8-2416-4CF4-AA0A-77819531DF15}"/>
-    <hyperlink ref="J13" r:id="rId124" tooltip="Supplier" display="'1655-1602-1-ND" xr:uid="{13BBE097-86BB-46AD-BF92-9097170A4C18}"/>
+    <hyperlink ref="G5" r:id="rId15" tooltip="Component" display="'Murata Electronics North America" xr:uid="{E7F5D5C7-EA41-4AA5-9366-4053E4BA72B3}"/>
+    <hyperlink ref="H5" r:id="rId16" tooltip="Manufacturer" display="'GRM32ER71H475KA88L" xr:uid="{A6EDC89B-1ED0-4754-9FF8-669DA8AF9522}"/>
+    <hyperlink ref="J5" r:id="rId17" tooltip="Supplier" display="'490-1864-1-ND" xr:uid="{A5AB9FC1-6372-4527-B577-FAA610CCDA97}"/>
+    <hyperlink ref="G9" r:id="rId18" tooltip="Component" display="'Diodes Inc" xr:uid="{2B3BD86C-29DA-46F2-8BAB-496617D12C1D}"/>
+    <hyperlink ref="H9" r:id="rId19" tooltip="Manufacturer" display="'S2BA-13-F" xr:uid="{28D5A782-892D-4B5B-8380-049E4BA9F589}"/>
+    <hyperlink ref="J9" r:id="rId20" tooltip="Supplier" display="'S2BA-FDICT-ND" xr:uid="{3F6CB655-0A7A-4880-A499-C0D848DB5627}"/>
+    <hyperlink ref="G10" r:id="rId21" tooltip="Component" display="'Micro Commercial Co" xr:uid="{0ABF9B14-67E4-403C-BC40-1631C6627605}"/>
+    <hyperlink ref="H10" r:id="rId22" tooltip="Manufacturer" display="'1N4148WX-TP" xr:uid="{E6239A4B-5131-49CD-92C9-030E55C8AD2E}"/>
+    <hyperlink ref="J10" r:id="rId23" tooltip="Supplier" display="'1N4148WXTPMSCT-ND" xr:uid="{4CBDC6BE-E0DC-495F-82C3-C420312D1A34}"/>
+    <hyperlink ref="G11" r:id="rId24" tooltip="Component" display="'Nexperia USA Inc." xr:uid="{1F61F94C-3850-4235-BC0F-EB9AD2F10894}"/>
+    <hyperlink ref="H11" r:id="rId25" tooltip="Manufacturer" display="'PMEG2020CPA,115" xr:uid="{0647B961-D44E-4662-B585-05AB6FA8A2CD}"/>
+    <hyperlink ref="J11" r:id="rId26" tooltip="Supplier" display="'1727-5194-1-ND" xr:uid="{25EBC6D0-7FBE-4D7E-8B6E-D589DB20F252}"/>
+    <hyperlink ref="G12" r:id="rId27" tooltip="Component" display="'Panasonic Electronic Components" xr:uid="{8E3BD2BA-DB6B-4FF3-A478-ACA69833B264}"/>
+    <hyperlink ref="H12" r:id="rId28" tooltip="Manufacturer" display="'DB2W40200L" xr:uid="{3761DF13-7813-4DFB-BC75-D47D9A3F904A}"/>
+    <hyperlink ref="J12" r:id="rId29" tooltip="Supplier" display="'DB2W40200LCT-ND" xr:uid="{48AE65F7-B989-4848-9591-2634A67A76AC}"/>
+    <hyperlink ref="G13" r:id="rId30" tooltip="Component" display="'SMC Diode Solutions" xr:uid="{AC22599F-B23D-4E43-AF11-EA72A9730063}"/>
+    <hyperlink ref="H13" r:id="rId31" tooltip="Manufacturer" display="'SK520BTR" xr:uid="{97298E20-975B-4CC3-8E21-71A6D4210AF9}"/>
+    <hyperlink ref="G14" r:id="rId32" tooltip="Component" display="'Sullins Connector Solutions" xr:uid="{F5FC59FA-9C19-4224-A7E5-E0FFF0CF83FE}"/>
+    <hyperlink ref="G15" r:id="rId33" tooltip="Component" display="'Phoenix Contact" xr:uid="{4766C111-E58E-4CDE-8EC1-5FBC0179B5E5}"/>
+    <hyperlink ref="H15" r:id="rId34" tooltip="Manufacturer" display="'1751264" xr:uid="{D31C62C5-0E89-49F5-9999-F164C1E7A95C}"/>
+    <hyperlink ref="J15" r:id="rId35" tooltip="Supplier" display="'277-5744-ND" xr:uid="{80E17885-8837-4CE3-93A1-C275271B3970}"/>
+    <hyperlink ref="G16" r:id="rId36" tooltip="Component" display="'Loading..." xr:uid="{DDFEE7F0-F3D2-4DC8-AE6C-7EAA9AFB0567}"/>
+    <hyperlink ref="G17" r:id="rId37" tooltip="Component" display="'Wurth Electronics Inc." xr:uid="{9C34FDB8-BE7F-40A9-9310-6F4073CE0FDF}"/>
+    <hyperlink ref="H17" r:id="rId38" tooltip="Manufacturer" display="'416131160803" xr:uid="{EC87D714-1A5E-4268-AF35-62693127FE37}"/>
+    <hyperlink ref="J17" r:id="rId39" tooltip="Supplier" display="'732-3853-1-ND" xr:uid="{87EF3683-C2E7-473B-868A-3A631DD27E52}"/>
+    <hyperlink ref="G18" r:id="rId40" tooltip="Component" display="'Loading..." xr:uid="{0A8E1813-F956-4A5B-8D10-B8DB52FDDBE4}"/>
+    <hyperlink ref="G19" r:id="rId41" tooltip="Component" display="'3M" xr:uid="{68CD3745-038B-4380-81BA-87034167EE3C}"/>
+    <hyperlink ref="G20" r:id="rId42" tooltip="Component" display="'MPD (Memory Protection Devices)" xr:uid="{FE298821-F0A5-4495-958A-5F81A2E04060}"/>
+    <hyperlink ref="H20" r:id="rId43" tooltip="Manufacturer" display="'BK-6013" xr:uid="{0F8C2023-4819-4C0C-B171-33CEE13AE4A6}"/>
+    <hyperlink ref="J20" r:id="rId44" tooltip="Supplier" display="'BK-6013-ND" xr:uid="{E61A265C-62CB-4F2B-942B-0CA0AF6703E9}"/>
+    <hyperlink ref="G21" r:id="rId45" tooltip="Component" display="'Holly Fuse" xr:uid="{0C8965CF-A757-4F40-A8B2-FD40A4E8C193}"/>
+    <hyperlink ref="H21" r:id="rId46" tooltip="Manufacturer" display="'06T-0160L" xr:uid="{87AB65B0-3F61-4B4B-BB53-75CD15E64701}"/>
+    <hyperlink ref="J21" r:id="rId47" tooltip="Supplier" display="'507-1821-1-ND" xr:uid="{EDCE14BF-745A-4FC1-B9D4-E74525915207}"/>
+    <hyperlink ref="G22" r:id="rId48" tooltip="Component" display="'Phoenix Contact" xr:uid="{8E33D070-85B3-45B0-9D72-9DEA8C64A27A}"/>
+    <hyperlink ref="H22" r:id="rId49" tooltip="Manufacturer" display="'1751248" xr:uid="{27069FCF-26AC-4F60-8EDA-B73F085A841F}"/>
+    <hyperlink ref="J22" r:id="rId50" tooltip="Supplier" display="'277-5719-ND" xr:uid="{072D2A82-ED4A-4927-B341-58FB066FBA76}"/>
+    <hyperlink ref="G48" r:id="rId51" tooltip="Component" display="'Loading..." xr:uid="{99534DDB-1774-407E-BD72-7D3668C9B630}"/>
+    <hyperlink ref="G24" r:id="rId52" tooltip="Component" display="'Loading..." xr:uid="{D760A977-B9E1-4C61-8FAE-CB62F2BEFBBD}"/>
+    <hyperlink ref="G25" r:id="rId53" tooltip="Component" display="'Molex, LLC" xr:uid="{0F5FD788-F564-4A60-A2B5-109732D6ED30}"/>
+    <hyperlink ref="H25" r:id="rId54" tooltip="Manufacturer" display="'1050170001" xr:uid="{B10606C0-E169-41AC-9B1B-F046E7E8510B}"/>
+    <hyperlink ref="J25" r:id="rId55" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{0989CB1B-579D-4020-A5FD-0E4ABE9D7703}"/>
+    <hyperlink ref="G26" r:id="rId56" tooltip="Component" display="'Murata Electronics North America" xr:uid="{D4304DAD-AEA9-4A0B-9023-C8C19E9FD2F3}"/>
+    <hyperlink ref="H26" r:id="rId57" tooltip="Manufacturer" display="'BLM21PG221SN1D" xr:uid="{63933F83-B76B-44CD-8CE8-1865C9C817D7}"/>
+    <hyperlink ref="J26" r:id="rId58" tooltip="Supplier" display="'490-1054-1-ND" xr:uid="{1E4D4793-B327-43AA-8F6C-D834CE45C90D}"/>
+    <hyperlink ref="G27" r:id="rId59" tooltip="Component" display="'Bourns Inc." xr:uid="{5E42FB16-A764-47DE-9A5B-D5B7FB62B66C}"/>
+    <hyperlink ref="H27" r:id="rId60" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{2CD86F8E-580A-44C3-A25C-C9769E024EF7}"/>
+    <hyperlink ref="J27" r:id="rId61" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{13951AE0-C7C0-43BA-BE32-C42CFD079DC4}"/>
+    <hyperlink ref="G28" r:id="rId62" tooltip="Component" display="'Bourns Inc." xr:uid="{3A3BA2F0-D76C-4591-8243-99CD334215D0}"/>
+    <hyperlink ref="H28" r:id="rId63" tooltip="Manufacturer" display="'SRN8040TA-470M" xr:uid="{9393FD5F-F406-4DDA-B2F6-A5087E59B162}"/>
+    <hyperlink ref="J28" r:id="rId64" tooltip="Supplier" display="'SRN8040TA-470MCT-ND" xr:uid="{BE956B5E-DBA7-4876-99D7-BD2953EE7A3E}"/>
+    <hyperlink ref="G29" r:id="rId65" tooltip="Component" display="'Lite-On Inc." xr:uid="{1BFC70D3-D369-4F4A-BC39-F51EC41C90E5}"/>
+    <hyperlink ref="H29" r:id="rId66" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{961D9B5D-F3D3-46C6-9E7D-993401706C55}"/>
+    <hyperlink ref="J29" r:id="rId67" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{4989D82B-EDE2-45AD-8316-0BE497E40D5B}"/>
+    <hyperlink ref="G30" r:id="rId68" tooltip="Component" display="'Lite-On Inc." xr:uid="{639D4ACD-5799-402D-803C-17A777CAFADE}"/>
+    <hyperlink ref="H30" r:id="rId69" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{2413BFA6-6008-41BC-AB9E-D0CADB0841F0}"/>
+    <hyperlink ref="J30" r:id="rId70" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{94979B37-F572-4850-BEF9-C3428194D2AD}"/>
+    <hyperlink ref="G33" r:id="rId71" tooltip="Component" display="'Yageo" xr:uid="{08B992B2-5FFD-468F-8C37-F5E0E55827CA}"/>
+    <hyperlink ref="H33" r:id="rId72" tooltip="Manufacturer" display="'RC0603FR-071ML" xr:uid="{7D006478-1E4D-4D42-85C7-033ABCB72197}"/>
+    <hyperlink ref="J33" r:id="rId73" tooltip="Supplier" display="'311-1.00MHRDKR-ND" xr:uid="{85B8248E-2152-4AEE-9145-234BD60567AA}"/>
+    <hyperlink ref="G36" r:id="rId74" tooltip="Component" display="'Yageo" xr:uid="{7A3BC117-10FA-4978-95C8-B8FEC528AE8C}"/>
+    <hyperlink ref="J36" r:id="rId75" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{6A20EF17-382F-49C2-A769-EBF46975E659}"/>
+    <hyperlink ref="G37" r:id="rId76" tooltip="Component" display="'Yageo" xr:uid="{5F9D81C6-4FA4-41B4-83FC-838B41BF9D63}"/>
+    <hyperlink ref="H37" r:id="rId77" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{EC5C9DBC-CA01-4E84-8AB1-A1E011F4969C}"/>
+    <hyperlink ref="J37" r:id="rId78" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{9EE26DE7-963D-4581-A9CD-06D42E170F76}"/>
+    <hyperlink ref="G39" r:id="rId79" tooltip="Component" display="'Yageo" xr:uid="{7CC16B12-D4DA-42BE-B00E-AF45B84234CE}"/>
+    <hyperlink ref="G41" r:id="rId80" tooltip="Component" display="'Yageo" xr:uid="{14BC76A9-9358-431A-80A8-D0CD2925110D}"/>
+    <hyperlink ref="H41" r:id="rId81" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{0C32B3D1-D5BC-425A-9128-C60912E9D570}"/>
+    <hyperlink ref="J41" r:id="rId82" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{F851E52C-EEB8-4A75-9E50-490FA833C07A}"/>
+    <hyperlink ref="G34" r:id="rId83" tooltip="Component" display="'Yageo" xr:uid="{04DAF956-9707-421B-9902-660D148AD02A}"/>
+    <hyperlink ref="H34" r:id="rId84" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{8885096B-1925-40B5-9B6A-8A913F04A0E5}"/>
+    <hyperlink ref="J34" r:id="rId85" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{008657BB-878C-496B-AC2C-CAF672731554}"/>
+    <hyperlink ref="G35" r:id="rId86" tooltip="Component" display="'Yageo" xr:uid="{2FBCF6ED-10E7-4215-9E32-249EF6E45BAE}"/>
+    <hyperlink ref="G38" r:id="rId87" tooltip="Component" display="'Yageo" xr:uid="{D05D8D23-0FD7-4EB0-82B5-012867FB4A29}"/>
+    <hyperlink ref="H38" r:id="rId88" tooltip="Manufacturer" display="'RC0603JR-074K7L" xr:uid="{487CC820-6958-4015-8E07-2B1B6917AB28}"/>
+    <hyperlink ref="J38" r:id="rId89" tooltip="Supplier" display="'311-4.7KGRCT-ND" xr:uid="{EB3C4C30-1438-46A2-85B2-C2570D6C8061}"/>
+    <hyperlink ref="G40" r:id="rId90" tooltip="Component" display="'Yageo" xr:uid="{83B23BCD-9D2D-4244-A8D9-855CBC334E2E}"/>
+    <hyperlink ref="H40" r:id="rId91" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{CC682DC2-92DA-4617-89AC-DBE9484E8EB3}"/>
+    <hyperlink ref="J40" r:id="rId92" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{77F80A98-4E5F-42FB-8366-09D154AF8FBF}"/>
+    <hyperlink ref="G42" r:id="rId93" tooltip="Component" display="'APEM Inc." xr:uid="{8DA80FE1-AD41-41A1-AF5B-29C7AE5C205A}"/>
+    <hyperlink ref="H42" r:id="rId94" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{3E38DB83-F083-4406-9B4E-413981B63A75}"/>
+    <hyperlink ref="J42" r:id="rId95" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{801CE691-B5ED-4969-8922-A4400E0A0F04}"/>
+    <hyperlink ref="G46" r:id="rId96" tooltip="Component" display="'Alpha &amp; Omega Semiconductor Inc." xr:uid="{B20D082B-86E0-455B-948A-E56AA2128005}"/>
+    <hyperlink ref="H46" r:id="rId97" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{FBD90C73-9CDC-45FA-A900-851BCE6704DB}"/>
+    <hyperlink ref="J46" r:id="rId98" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{E2C42AC0-6C55-40A7-8049-274675441D9B}"/>
+    <hyperlink ref="G47" r:id="rId99" tooltip="Component" display="'STMicroelectronics" xr:uid="{785209C2-D378-474E-97B4-42C17DE72E9A}"/>
+    <hyperlink ref="H47" r:id="rId100" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{98791FDC-D4C5-4551-847A-1B45F6539CBF}"/>
+    <hyperlink ref="J47" r:id="rId101" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{E2F9A172-96B8-4383-B884-A6A1414CF4A7}"/>
+    <hyperlink ref="G43" r:id="rId102" tooltip="Component" display="'Microchip Technology" xr:uid="{D0D2B9E1-7600-421F-BB55-D5E4CF817D2B}"/>
+    <hyperlink ref="H43" r:id="rId103" tooltip="Manufacturer" display="'ATMEGA2560-16AU" xr:uid="{3090BB5A-0847-4847-AA65-518ED9057C4F}"/>
+    <hyperlink ref="J43" r:id="rId104" tooltip="Supplier" display="'ATMEGA2560-16AU-ND" xr:uid="{21D45919-A9D2-4071-80EE-68A0A0D8492D}"/>
+    <hyperlink ref="G44" r:id="rId105" tooltip="Component" display="'Microchip Technology" xr:uid="{21BB9AC5-9AC5-4C89-A6B2-5C2DD94EEA56}"/>
+    <hyperlink ref="H44" r:id="rId106" tooltip="Manufacturer" display="'ATMEGA16U2-AU" xr:uid="{71DEC28B-A006-4DF5-BB66-FBB703DC7EFC}"/>
+    <hyperlink ref="J44" r:id="rId107" tooltip="Supplier" display="'ATMEGA16U2-AU-ND" xr:uid="{752CFA2A-364D-4706-BD90-0EF7750AEE11}"/>
+    <hyperlink ref="G45" r:id="rId108" tooltip="Component" display="'Alpha &amp; Omega Semiconductor Inc." xr:uid="{BE4F2880-1B87-45DB-B4B9-3BC68B11948D}"/>
+    <hyperlink ref="H45" r:id="rId109" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{00CF3BA0-9B64-4C44-A4CC-99B3C12958E9}"/>
+    <hyperlink ref="J45" r:id="rId110" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{CE07DCE4-81F1-4E37-AE55-1FF5C4A25DD5}"/>
+    <hyperlink ref="G49" r:id="rId111" tooltip="Component" display="'Loading..." xr:uid="{7FFD9829-C7FD-48AB-9008-67414D5F3A9B}"/>
+    <hyperlink ref="G50" r:id="rId112" tooltip="Component" display="'EPSON" xr:uid="{307A7C81-BA6D-4A04-84C8-3CD77AE1DB8E}"/>
+    <hyperlink ref="H50" r:id="rId113" tooltip="Manufacturer" display="'FA-238 16.0000MB-C3" xr:uid="{38323FE7-4E4F-4998-8A1E-5F7113325831}"/>
+    <hyperlink ref="J50" r:id="rId114" tooltip="Supplier" display="'SER3686CT-ND" xr:uid="{225B874A-BB17-40EC-AD86-2ADBDA9439C8}"/>
+    <hyperlink ref="G32" r:id="rId115" tooltip="Component" xr:uid="{8C0B0BB1-B33C-4761-A4B1-3E86C1AAAB94}"/>
+    <hyperlink ref="H32" r:id="rId116" tooltip="Manufacturer" xr:uid="{6F8EF1F8-2416-4CF4-AA0A-77819531DF15}"/>
+    <hyperlink ref="J13" r:id="rId117" tooltip="Supplier" display="'1655-1602-1-ND" xr:uid="{13BBE097-86BB-46AD-BF92-9097170A4C18}"/>
+    <hyperlink ref="H36" r:id="rId118" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{3E10DF3F-5206-4953-A38F-24F8BF7A0D63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="219" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId125"/>
+  <pageSetup paperSize="219" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId119"/>
   <tableParts count="1">
-    <tablePart r:id="rId126"/>
+    <tablePart r:id="rId120"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>